<commit_message>
another ghost hunter replay
</commit_message>
<xml_diff>
--- a/ghost-hunter/checklist.xlsx
+++ b/ghost-hunter/checklist.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/ghost-hunter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49E56A2-452A-8D41-8D7C-4FB0BB5DF353}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F77A5FD-5372-454F-B87C-E450D8CE8B3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{6AA9269F-948D-DB47-88FF-78A622A1EF45}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>year</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>Aspect</t>
+  </si>
+  <si>
+    <t>ゴーストハンターRPG02リプレイ 黒き死の仮面―草壁健一郎の事件簿</t>
+  </si>
+  <si>
+    <t>Ghost Hunter RPG02 Replay Black Death Mask-Kenichiro Kusakabe's Casebook</t>
+  </si>
+  <si>
+    <t>Fujimi Shobo</t>
+  </si>
+  <si>
+    <t>black-death-mask-replay2.jpg</t>
   </si>
 </sst>
 </file>
@@ -501,16 +513,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30072C2B-0790-4742-8047-1B90A8F0DBAC}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="59.1640625" customWidth="1"/>
+    <col min="2" max="2" width="72.83203125" customWidth="1"/>
     <col min="3" max="3" width="52.5" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
@@ -636,43 +648,63 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2003</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2003</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>